<commit_message>
Updated KTH_car_experiment values and parameters
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/AutowareConfig1.xlsx
+++ b/AD-EYE/TA/AutowareConfig1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96D2186-83DA-414D-A8F3-582F6D60795A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A60874C-4665-47FA-A9F9-1E509BB2034C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2055" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1138,7 +1138,7 @@
   </sheetPr>
   <dimension ref="A1:G239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G169" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A169" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G196" sqref="G196"/>
     </sheetView>
   </sheetViews>
@@ -5230,7 +5230,7 @@
         <v>50</v>
       </c>
       <c r="G195" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Car Experiment ranges (distance and speed)
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/AutowareConfig1.xlsx
+++ b/AD-EYE/TA/AutowareConfig1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A60874C-4665-47FA-A9F9-1E509BB2034C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DA75FC-6192-4FB1-AF11-8EEC13C35E8F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1138,8 +1138,8 @@
   </sheetPr>
   <dimension ref="A1:G239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G196" sqref="G196"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,7 +1482,7 @@
         <v>3</v>
       </c>
       <c r="G15" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>